<commit_message>
CIPW last check + collecting usig data in one map
- all the usefull data i put away in one folder (it was a little bit confusing with all the files with different names)
</commit_message>
<xml_diff>
--- a/_CIPW/QAPF_count.xlsx
+++ b/_CIPW/QAPF_count.xlsx
@@ -380,110 +380,108 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2743</v>
+        <v>3783</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>granodiorite</t>
+          <t>quartz monzonite</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1212</v>
+        <v>549</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
+          <t>syeno granite</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>granodiorite</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>quartz syenite</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>monzonite</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
           <t>quartz monzodiorite
 quartz monzogabbro</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>quartz monzonite</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>tonalite</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>monzodiorite monzogabbro</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>syeno granite</t>
-        </is>
-      </c>
       <c r="B8" t="n">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>quartz diorite
-quartz gabbro
-quartz anorthosite</t>
+          <t>quartz-rich granitoid</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>monzonite</t>
+          <t>syenite</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>diorite gabbro anorthosite</t>
+          <t>tonalite</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>quartz-rich granitoid</t>
+          <t>monzodiorite monzogabbro</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>